<commit_message>
tabla prestamo agregue 10 quincena al monto de 10000
</commit_message>
<xml_diff>
--- a/tabla de prestamos.xlsx
+++ b/tabla de prestamos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personales\utilitario\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7620"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,12 +41,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,7 +89,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -94,14 +99,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,28 +377,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>3000</v>
       </c>
@@ -416,7 +421,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3000</v>
       </c>
@@ -427,11 +432,11 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5000</v>
       </c>
@@ -442,7 +447,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5000</v>
       </c>
@@ -453,7 +458,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5000</v>
       </c>
@@ -464,11 +469,11 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>10000</v>
       </c>
@@ -479,7 +484,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10000</v>
       </c>
@@ -490,7 +495,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10000</v>
       </c>
@@ -501,7 +506,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10000</v>
       </c>
@@ -512,160 +517,171 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>10000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="5">
-        <v>3000</v>
-      </c>
-      <c r="B16" s="1">
-        <v>4</v>
-      </c>
-      <c r="C16" s="4">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>3000</v>
       </c>
       <c r="B17" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C17" s="4">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>3000</v>
       </c>
       <c r="B18" s="1">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>3000</v>
+      </c>
+      <c r="B19" s="1">
         <v>8</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C19" s="4">
         <v>450</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5">
-        <v>5000</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>5000</v>
+      </c>
+      <c r="B21" s="1">
         <v>4</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C21" s="4">
         <v>1375</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="5">
-        <v>5000</v>
-      </c>
-      <c r="B21" s="1">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>5000</v>
+      </c>
+      <c r="B22" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C22" s="4">
         <v>960</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="5">
-        <v>5000</v>
-      </c>
-      <c r="B22" s="1">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>5000</v>
+      </c>
+      <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C23" s="4">
         <v>750</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5">
-        <v>5000</v>
-      </c>
-      <c r="B23" s="1">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>5000</v>
+      </c>
+      <c r="B24" s="1">
         <v>10</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C24" s="4">
         <v>625</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5">
-        <v>5000</v>
-      </c>
-      <c r="B24" s="1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>5000</v>
+      </c>
+      <c r="B25" s="1">
         <v>12</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C25" s="4">
         <v>540</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5">
-        <v>10000</v>
-      </c>
-      <c r="B26" s="1">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>10000</v>
+      </c>
+      <c r="B27" s="1">
         <v>4</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C27" s="4">
         <v>2750</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="5">
-        <v>10000</v>
-      </c>
-      <c r="B27" s="1">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>10000</v>
+      </c>
+      <c r="B28" s="1">
         <v>6</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C28" s="4">
         <v>1920</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="5">
-        <v>10000</v>
-      </c>
-      <c r="B28" s="1">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>10000</v>
+      </c>
+      <c r="B29" s="1">
         <v>8</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C29" s="4">
         <v>1500</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="5">
-        <v>10000</v>
-      </c>
-      <c r="B29" s="1">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>10000</v>
+      </c>
+      <c r="B30" s="1">
         <v>10</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C30" s="4">
         <v>1250</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5">
-        <v>10000</v>
-      </c>
-      <c r="B30" s="1">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>10000</v>
+      </c>
+      <c r="B31" s="1">
         <v>12</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C31" s="4">
         <v>1090</v>
       </c>
     </row>

</xml_diff>